<commit_message>
Add skills for each project in project page
- Add main skills to each project's data
- Add skills to SingleProject element
- Improve styling to single project's skills
</commit_message>
<xml_diff>
--- a/src/assets/files/Media Breakpoints Style Map.xlsx
+++ b/src/assets/files/Media Breakpoints Style Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Work\Web Dev\Projects\Personal Projects\Portfolio Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Work\Web Dev\Projects\Personal Projects\Portfolio Website\portfolio-website\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE0F699-0A66-48DD-9015-23EC64CDE5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF38607-0D9F-4C76-BB2B-642E6702383D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3924" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Improve profile picture and responsiveness
- Add images for new profile picture, skill logos and project thumbnails
- Add new resume file
- Change app's homepage name to "brunomiguel"
- Update 'browserslist' in package.json to improve app responsiveness in production
- Update homepage profile picture
- Update Readme
- Improve "About" page's styling and responsiveness
- Add new description and server code button to "Buzz Circle" project in "Projects" page
- Improve "Projects" page styling and responsiveness
- Improve burger menu styling on mobile screens
- Add a script to the public/index.html file and add a public/404.html file with a script to work around the GitHub Pages bug where it displays "404" page upon page refresh in a URL that's not the homepage URL
</commit_message>
<xml_diff>
--- a/src/assets/files/Media Breakpoints Style Map.xlsx
+++ b/src/assets/files/Media Breakpoints Style Map.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Work\Web Dev\Projects\Personal Projects\Portfolio Website\portfolio-website\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80A1524-50E7-4179-9C38-89D29C1EAB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE0E075-1C41-43B8-B25E-159F66558081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11544" yWindow="-17280" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11544" yWindow="-17280" windowWidth="15360" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -590,7 +589,7 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>